<commit_message>
Make add new student and write excel
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/bin/Debug/Database.xlsx
+++ b/WindowsFormsApp2/bin/Debug/Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duy minh\source\repos\WindowsFormsApp1\WindowsFormsApp1\QLSV_Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duy minh\source\repos\WindowsFormsApp1\WindowsFormsApp1\WindowsFormsApp2\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SinhVien" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="TOTNGHIEP">SinhVien!$G$4</definedName>
+    <definedName name="TOTNGHIEP">SinhVien!$I$4</definedName>
   </definedNames>
   <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
@@ -29,7 +29,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <si>
+    <t>Lê Quang Duy Minh</t>
+  </si>
+  <si>
+    <t>Huỳnh Hải Đăng</t>
+  </si>
+  <si>
+    <t>17CT11</t>
+  </si>
+  <si>
+    <t>17CT12</t>
+  </si>
+  <si>
+    <t>a123456</t>
+  </si>
+  <si>
+    <t>b123456</t>
+  </si>
+  <si>
+    <t>NAM</t>
+  </si>
+  <si>
+    <t>NU</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>ngokgnekboy@gmail.com</t>
+  </si>
+  <si>
+    <t>helloboy@gmail.com</t>
+  </si>
+  <si>
+    <t>btx Tỉnh Đồng Nai</t>
+  </si>
+  <si>
+    <t>Tỉnh Bình Dương</t>
+  </si>
   <si>
     <t>CT</t>
   </si>
@@ -61,73 +103,31 @@
     <t>Đông Phương Học</t>
   </si>
   <si>
-    <t>Lê Quang Duy Minh</t>
-  </si>
-  <si>
-    <t>Huỳnh Hải Đăng</t>
+    <t>17CT1</t>
   </si>
   <si>
     <t>Cong Nghe Thong Tin 1</t>
   </si>
   <si>
+    <t>17CT2</t>
+  </si>
+  <si>
     <t>Cong Nghe Thong Tin 2</t>
   </si>
   <si>
+    <t>17CT3</t>
+  </si>
+  <si>
     <t>Cong Nghe Thong Tin 3</t>
   </si>
   <si>
-    <t>17CT11</t>
-  </si>
-  <si>
-    <t>17CT12</t>
-  </si>
-  <si>
-    <t>17CT1</t>
-  </si>
-  <si>
-    <t>17CT2</t>
-  </si>
-  <si>
-    <t>17CT3</t>
-  </si>
-  <si>
-    <t>a123456</t>
-  </si>
-  <si>
-    <t>b123456</t>
-  </si>
-  <si>
-    <t>NAM</t>
-  </si>
-  <si>
-    <t>NU</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>ngokgnekboy@gmail.com</t>
-  </si>
-  <si>
-    <t>helloboy@gmail.com</t>
-  </si>
-  <si>
-    <t>Huỳnh Hải Dũng</t>
-  </si>
-  <si>
-    <t>btx Tỉnh Đồng Nai</t>
-  </si>
-  <si>
-    <t>Tỉnh Bình Dương</t>
-  </si>
-  <si>
-    <t>Cà Mau</t>
-  </si>
-  <si>
-    <t>helloboy1@gmail.com</t>
+    <t>dasd</t>
+  </si>
+  <si>
+    <t>42134a</t>
+  </si>
+  <si>
+    <t>a312312</t>
   </si>
 </sst>
 </file>
@@ -172,11 +172,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,7 +462,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,43 +471,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -519,7 +520,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,10 +533,10 @@
         <v>2017</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -543,10 +544,10 @@
         <v>2017</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -554,10 +555,10 @@
         <v>2017</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -567,10 +568,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,102 +580,95 @@
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="50.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C1">
         <v>767350000</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1">
         <v>34857</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>33213123</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1">
         <v>36526</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3">
-        <v>33213123</v>
+        <v>312</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="E3"/>
       <c r="F3" s="1">
-        <v>36526</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="3" t="s">
+        <v>44120.787280092591</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E4"/>
+      <c r="G4" s="1"/>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I1" r:id="rId1"/>
-    <hyperlink ref="I2" r:id="rId2"/>
-    <hyperlink ref="I3" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hi hi do ngok
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/bin/Debug/Database.xlsx
+++ b/WindowsFormsApp2/bin/Debug/Database.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duy minh\source\repos\WindowsFormsApp1\WindowsFormsApp1\WindowsFormsApp2\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dangh\OneDrive\Documents\GitHub\ProjectQLSV_Final_18CT113\WindowsFormsApp2\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Khoa" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Lê Quang Duy Minh</t>
   </si>
@@ -517,10 +517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +528,7 @@
     <col min="3" max="3" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2017</v>
       </c>
@@ -538,8 +538,11 @@
       <c r="C1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2017</v>
       </c>
@@ -549,8 +552,11 @@
       <c r="C2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2017</v>
       </c>
@@ -559,6 +565,9 @@
       </c>
       <c r="C3" t="s">
         <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -568,10 +577,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,15 +588,15 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>118001525</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -613,10 +622,13 @@
       <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>118001526</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -642,8 +654,14 @@
       <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>118001527</v>
+      </c>
       <c r="B3" t="s">
         <v>30</v>
       </c>
@@ -663,7 +681,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E4"/>
       <c r="G4" s="1"/>
     </row>

</xml_diff>

<commit_message>
hello thay, em lam ne. HIHI ^^
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/bin/Debug/Database.xlsx
+++ b/WindowsFormsApp2/bin/Debug/Database.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>Lê Quang Duy Minh</t>
   </si>
@@ -140,6 +140,18 @@
   </si>
   <si>
     <t>quy oc cho</t>
+  </si>
+  <si>
+    <t>Nu</t>
+  </si>
+  <si>
+    <t>ddsadas</t>
+  </si>
+  <si>
+    <t>dsa</t>
+  </si>
+  <si>
+    <t>dsadas</t>
   </si>
 </sst>
 </file>
@@ -589,10 +601,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,8 +699,12 @@
       <c r="F3" s="1">
         <v>44120.787280092591</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="I3" t="s">
         <v>30</v>
       </c>
@@ -713,7 +729,12 @@
       <c r="F4" s="1">
         <v>44120.787280092591</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
       <c r="I4" t="s">
         <v>33</v>
       </c>
@@ -734,8 +755,37 @@
       <c r="F5" s="1">
         <v>44120.787280092591</v>
       </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
       <c r="I5" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="1">
+        <v>44120.787280092591</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update search sinhvien and push data into datagridviewSinhVien
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/bin/Debug/Database.xlsx
+++ b/WindowsFormsApp2/bin/Debug/Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dangh\OneDrive\Documents\GitHub\ProjectQLSV_Final_18CT113\WindowsFormsApp2\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duy minh\Documents\GitHub\ProjectQLSV_Final_18CT113\WindowsFormsApp2\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
   <si>
     <t>Lê Quang Duy Minh</t>
   </si>
@@ -601,10 +601,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,6 +788,115 @@
         <v>40</v>
       </c>
     </row>
+    <row r="7" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>118001525</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>767350000</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>34857</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>118001526</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>33213123</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>36526</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>118001527</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4">
+        <v>312</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1">
+        <v>44120.787280092591</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="2"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+      <c r="F13" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix upgrade data sv
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/bin/Debug/Database.xlsx
+++ b/WindowsFormsApp2/bin/Debug/Database.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
   <si>
     <t>Lê Quang Duy Minh</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>20CT2</t>
+  </si>
+  <si>
+    <t>wsq</t>
   </si>
 </sst>
 </file>
@@ -781,15 +784,17 @@
       <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="E3"/>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
       <c r="F3" s="7">
-        <v>44120.787280092591</v>
+        <v>44120</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Update Task Lop (Print report)
Done by Minh
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/bin/Debug/Database.xlsx
+++ b/WindowsFormsApp2/bin/Debug/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Khoa" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
   <si>
     <t>Lê Quang Duy Minh</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>NU</t>
-  </si>
-  <si>
-    <t>YES</t>
   </si>
   <si>
     <t>NO</t>
@@ -557,42 +554,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -604,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -618,13 +615,13 @@
         <v>2017</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,13 +629,13 @@
         <v>2017</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -646,13 +643,13 @@
         <v>2017</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -660,13 +657,13 @@
         <v>2020</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -674,13 +671,13 @@
         <v>2020</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -692,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +715,7 @@
         <v>767350000</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -733,10 +730,10 @@
         <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -750,7 +747,7 @@
         <v>33213123</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
@@ -759,16 +756,16 @@
         <v>36526</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -776,28 +773,28 @@
         <v>18001527</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="7">
         <v>44120</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -805,13 +802,13 @@
         <v>18001523</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>767350000</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -826,10 +823,10 @@
         <v>4</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -837,13 +834,13 @@
         <v>18001520</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>33213123</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
@@ -852,16 +849,16 @@
         <v>36526</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -869,28 +866,28 @@
         <v>18001534</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>312</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="7">
         <v>44120.787280092591</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H6" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -898,26 +895,26 @@
         <v>18000923</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4">
         <v>321312</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="7">
         <v>44120.787280092591</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -925,26 +922,26 @@
         <v>18000923</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4">
         <v>321312</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="7">
         <v>44120.787280092591</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -952,25 +949,25 @@
         <v>18000923</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="4">
         <v>3213</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="7">
         <v>44120.787280092591</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -978,13 +975,13 @@
         <v>20000001</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="4">
         <v>3213</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>2</v>
@@ -993,13 +990,13 @@
         <v>44120.787280092591</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1007,13 +1004,13 @@
         <v>20000002</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="4">
         <v>312</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>2</v>
@@ -1022,13 +1019,13 @@
         <v>44120.787280092591</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1036,13 +1033,13 @@
         <v>20000003</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4">
         <v>312</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>2</v>
@@ -1051,16 +1048,16 @@
         <v>44120.787280092591</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1068,13 +1065,13 @@
         <v>20000005</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="4">
         <v>312</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>2</v>
@@ -1083,16 +1080,16 @@
         <v>44120</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Phân Lớp Giáo Viên
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/bin/Debug/Database.xlsx
+++ b/WindowsFormsApp2/bin/Debug/Database.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Khoa" sheetId="1" r:id="rId1"/>
     <sheet name="Lop" sheetId="2" r:id="rId2"/>
     <sheet name="SinhVien" sheetId="3" r:id="rId3"/>
     <sheet name="NamHoc" sheetId="4" r:id="rId4"/>
+    <sheet name="GiaoVien" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="TOTNGHIEP">SinhVien!$I$4</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
   <si>
     <t>Lê Quang Duy Minh</t>
   </si>
@@ -207,13 +208,70 @@
   </si>
   <si>
     <t>wsq</t>
+  </si>
+  <si>
+    <t>Hùng</t>
+  </si>
+  <si>
+    <t>Dũng</t>
+  </si>
+  <si>
+    <t>Minh</t>
+  </si>
+  <si>
+    <t>Đăng</t>
+  </si>
+  <si>
+    <t>Quý</t>
+  </si>
+  <si>
+    <t>Óc</t>
+  </si>
+  <si>
+    <t>dung@gmail.com</t>
+  </si>
+  <si>
+    <t>dang@gmail.com</t>
+  </si>
+  <si>
+    <t>quy@gmail.com</t>
+  </si>
+  <si>
+    <t>hung@gmail.com</t>
+  </si>
+  <si>
+    <t>minh@gmail.com</t>
+  </si>
+  <si>
+    <t>oc@gmail.com</t>
+  </si>
+  <si>
+    <t>GV1</t>
+  </si>
+  <si>
+    <t>GV2</t>
+  </si>
+  <si>
+    <t>GV3</t>
+  </si>
+  <si>
+    <t>GV4</t>
+  </si>
+  <si>
+    <t>GV5</t>
+  </si>
+  <si>
+    <t>GV6</t>
+  </si>
+  <si>
+    <t>1234a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +281,20 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -251,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -260,6 +332,8 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -599,10 +673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +684,7 @@
     <col min="3" max="3" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2017</v>
       </c>
@@ -623,8 +697,11 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2017</v>
       </c>
@@ -637,8 +714,11 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2017</v>
       </c>
@@ -651,8 +731,11 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -665,8 +748,11 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2020</v>
       </c>
@@ -678,6 +764,9 @@
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -689,7 +778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -874,8 +963,11 @@
       <c r="D6" t="s">
         <v>27</v>
       </c>
+      <c r="E6" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="F6" s="7">
-        <v>44120.787280092591</v>
+        <v>44120</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
@@ -1282,4 +1374,88 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.28515625" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Đổi Mật Khẩu, Thêm Lớp, Phân Công Giáo Viên, GIao Diện User
Update Đổi Mật Khẩu, Thêm Lớp, Phân Công Giáo Viên, Hiện Danh Sách SV của Lớp,GIao Diện User
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/bin/Debug/Database.xlsx
+++ b/WindowsFormsApp2/bin/Debug/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Khoa" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="SinhVien" sheetId="3" r:id="rId3"/>
     <sheet name="NamHoc" sheetId="4" r:id="rId4"/>
     <sheet name="GiaoVien" sheetId="6" r:id="rId5"/>
+    <sheet name="Admin" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="TOTNGHIEP">SinhVien!$I$4</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
   <si>
     <t>Lê Quang Duy Minh</t>
   </si>
@@ -138,24 +139,6 @@
     <t>ds321312@gmail.com</t>
   </si>
   <si>
-    <t>Con Ga</t>
-  </si>
-  <si>
-    <t>chuong ga</t>
-  </si>
-  <si>
-    <t>dsadas@gmail.com</t>
-  </si>
-  <si>
-    <t>Con Vit</t>
-  </si>
-  <si>
-    <t>chuong vbit</t>
-  </si>
-  <si>
-    <t>")312</t>
-  </si>
-  <si>
     <t>lOI</t>
   </si>
   <si>
@@ -168,15 +151,6 @@
     <t>20CT1</t>
   </si>
   <si>
-    <t>duy</t>
-  </si>
-  <si>
-    <t>minh321</t>
-  </si>
-  <si>
-    <t>dsa</t>
-  </si>
-  <si>
     <t>asd</t>
   </si>
   <si>
@@ -265,6 +239,30 @@
   </si>
   <si>
     <t>1234a</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>dasd12421</t>
+  </si>
+  <si>
+    <t>a123456ds</t>
+  </si>
+  <si>
+    <t>20CT3</t>
+  </si>
+  <si>
+    <t>17EE1</t>
+  </si>
+  <si>
+    <t>Xây Dựng 1</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin2</t>
   </si>
 </sst>
 </file>
@@ -673,10 +671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +696,7 @@
         <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -715,7 +713,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -732,7 +730,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -740,7 +738,7 @@
         <v>2020</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -749,7 +747,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -757,7 +755,7 @@
         <v>2020</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>24</v>
@@ -766,7 +764,41 @@
         <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2020</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2017</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -779,7 +811,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +854,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -871,7 +903,7 @@
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F3" s="7">
         <v>44120</v>
@@ -906,7 +938,7 @@
         <v>34857</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -938,7 +970,7 @@
         <v>36526</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="H5" t="s">
         <v>5</v>
@@ -964,7 +996,7 @@
         <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F6" s="7">
         <v>44120</v>
@@ -990,14 +1022,16 @@
         <v>35</v>
       </c>
       <c r="C7" s="4">
-        <v>321312</v>
+        <v>3213</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="F7" s="7">
-        <v>44120.787280092591</v>
+        <v>44120</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>6</v>
@@ -1011,20 +1045,22 @@
     </row>
     <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>18000923</v>
+        <v>20000002</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4">
-        <v>321312</v>
+        <v>312</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="F8" s="7">
-        <v>44120.787280092591</v>
+        <v>44120</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>6</v>
@@ -1033,24 +1069,27 @@
         <v>4</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>18000923</v>
+        <v>20000003</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4">
-        <v>3213</v>
+        <v>312</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="F9" s="7">
-        <v>44120.787280092591</v>
+        <v>44120</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>6</v>
@@ -1059,27 +1098,30 @@
         <v>4</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>20000001</v>
+        <v>20000005</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="4">
+        <v>312</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" s="4">
-        <v>3213</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F10" s="7">
-        <v>44120.787280092591</v>
+        <v>44120</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>6</v>
@@ -1088,101 +1130,24 @@
         <v>4</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>20000002</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="4">
-        <v>312</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="7">
-        <v>44120.787280092591</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>20000003</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="4">
-        <v>312</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="7">
-        <v>44120.787280092591</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>20000005</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="4">
-        <v>312</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="7">
-        <v>44120</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="5"/>
@@ -1198,7 +1163,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,70 +1354,119 @@
     <col min="3" max="3" width="21.28515625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Check Email Trùng, Danh Sách SV Của Giáo Viên CN, Danh Sách SV của từng Lớp, Quên Mật Khẩu
Check Email Trùng, Danh Sách SV Của Giáo Viên CN, Danh Sách SV của từng Lớp, Quên Mật Khẩu
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/bin/Debug/Database.xlsx
+++ b/WindowsFormsApp2/bin/Debug/Database.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="84">
   <si>
     <t>Lê Quang Duy Minh</t>
   </si>
@@ -263,6 +263,27 @@
   </si>
   <si>
     <t>admin2</t>
+  </si>
+  <si>
+    <t>va anh</t>
+  </si>
+  <si>
+    <t>dsadsa@gmail.com</t>
+  </si>
+  <si>
+    <t>20EE1</t>
+  </si>
+  <si>
+    <t>20EE2</t>
+  </si>
+  <si>
+    <t>Xây Dựng 2</t>
+  </si>
+  <si>
+    <t>das@gmail.com</t>
+  </si>
+  <si>
+    <t>sad@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -671,7 +692,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -801,6 +822,34 @@
         <v>67</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2020</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2020</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -811,7 +860,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,8 +1012,8 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>3</v>
+      <c r="E5" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="F5" s="7">
         <v>36526</v>
@@ -1137,8 +1186,36 @@
       </c>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="2"/>
-      <c r="F11" s="7"/>
+      <c r="A11" s="4">
+        <v>20000006</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="4">
+        <v>734</v>
+      </c>
+      <c r="D11" s="5">
+        <v>43873</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="7">
+        <v>43767</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E12" s="2"/>
@@ -1197,7 +1274,7 @@
         <v>2020</v>
       </c>
       <c r="B4" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1346,7 +1423,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1441,7 @@
       <c r="C1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1445,28 +1522,37 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>